<commit_message>
New articles on sources of plastic
</commit_message>
<xml_diff>
--- a/Source Links.xlsx
+++ b/Source Links.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kalyj\Google Drive\RGU\MSc Data Science\CMM507 - Research Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kalyj\OneDrive\RGU\MSc Data Science\CMM507Group2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A19774D1-690D-4199-B5B3-708A58596579}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="8_{A19774D1-690D-4199-B5B3-708A58596579}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3F3D3CCB-ABCC-47B5-BFF0-5DF7AF0D37C6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="21816" windowHeight="14016" xr2:uid="{DEE519DF-CA73-4E24-A15D-8AAE2AE5105B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="64">
   <si>
     <t>Link</t>
   </si>
@@ -69,6 +69,182 @@
   </si>
   <si>
     <t>Roshi</t>
+  </si>
+  <si>
+    <t>https://www.weforum.org/agenda/2018/06/90-of-plastic-polluting-our-oceans-comes-from-just-10-rivers/</t>
+  </si>
+  <si>
+    <t>Karen</t>
+  </si>
+  <si>
+    <t>Sources of plastic pollution</t>
+  </si>
+  <si>
+    <t>https://www.pnas.org/content/116/42/20892</t>
+  </si>
+  <si>
+    <t>Stuart</t>
+  </si>
+  <si>
+    <t>https://journals.plos.org/plosone/article?id=10.1371/journal.pone.0080466#s5</t>
+  </si>
+  <si>
+    <t>accumulation zones</t>
+  </si>
+  <si>
+    <t>Georgios</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0025326X11005674</t>
+  </si>
+  <si>
+    <t>plastic density - weight &amp; count (dataset)</t>
+  </si>
+  <si>
+    <t>https://www.nationalgeographic.co.uk/environment-and-conservation/2019/08/what-its-swim-through-great-pacific-garbage-patch</t>
+  </si>
+  <si>
+    <t>Vortex swim</t>
+  </si>
+  <si>
+    <t>https://pubs.acs.org/doi/10.1021/acs.est.7b02368</t>
+  </si>
+  <si>
+    <t>non-scientific article referencing "Export of Plastic Debris by Rivers into the Sea"</t>
+  </si>
+  <si>
+    <t>Sources of plastic pollution. (dataset) + bibtech ref</t>
+  </si>
+  <si>
+    <t>http://jambeck.engr.uga.edu/landplasticinput</t>
+  </si>
+  <si>
+    <t>Export of Plastic Debris by Rivers into the Sea
+Christian Schmidt, Tobias Krauth, and Stephan Wagner (2017)
+Environmental Science &amp; Technology 2017 51 (21), 12246-12253
+DOI: 10.1021/acs.est.7b02368</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plastic waste inputs from land into the ocean, Science, 347, p. 768-771. Jambeck, J.R., Andrady, A., Geyer, R., Narayan, R., Perryman, M., Siegler, T., Wilcox, C., Lavender Law, K. , (2015). </t>
+  </si>
+  <si>
+    <t>https://advances.sciencemag.org/content/3/7/e1700782.short</t>
+  </si>
+  <si>
+    <t>Production, use, and fate of all plastics ever made
+BY ROLAND GEYER, JENNA R. JAMBECK, KARA LAVENDER LAW
+SCIENCE ADVANCES19 JUL 2017 : E1700782</t>
+  </si>
+  <si>
+    <t>Sources of plastic pollution.</t>
+  </si>
+  <si>
+    <t>https://www.nationalgeographic.com/news/2017/07/plastic-produced-recycling-waste-ocean-trash-debris-environment/</t>
+  </si>
+  <si>
+    <t>non-scientific article referencing "Production, use, and fate of all plastics ever made"</t>
+  </si>
+  <si>
+    <t>https://www.nature.com/articles/s41467-019-09506-1</t>
+  </si>
+  <si>
+    <t>The rise in ocean plastics evidenced from a 60-year time series. Nat Commun 10, 1622
+Ostle, C., Thompson, R.C., Broughton, D. et al.  (2019). https://doi.org/10.1038/s41467-019-09506-1</t>
+  </si>
+  <si>
+    <t>(dataset) somewhere</t>
+  </si>
+  <si>
+    <t>https://journals.plos.org/plosone/article?id=10.1371/journal.pone.0111913</t>
+  </si>
+  <si>
+    <t>Plastic Pollution in the World's Oceans: More than 5 Trillion Plastic Pieces Weighing over 250,000 Tons Afloat at Sea
+Marcus Eriksen ,Laurent C. M. Lebreton,Henry S. Carson,Martin Thiel,Charles J. Moore,Jose C. Borerro,Francois Galgani,Peter G. Ryan,Julia Reisser
+Published: December 10, 2014https://doi.org/10.1371/journal.pone.0111913</t>
+  </si>
+  <si>
+    <t>dataset in https://www.arcgis.com/home/item.html?id=0a84536e5172481c971f6b81c49d3b3e</t>
+  </si>
+  <si>
+    <t>https://iopscience.iop.org/article/10.1088/1748-9326/7/4/044040</t>
+  </si>
+  <si>
+    <t>Origin, dynamics and evolution of ocean garbage patches from observed surface drifters
+Erik van Sebille Matthew H England and Gary Froyland
+Published 19 December 2012 • 2012 IOP Publishing Ltd
+Environmental Research Letters, Volume 7, Number 4</t>
+  </si>
+  <si>
+    <t>Rapid increase in Asian bottles in the South Atlantic Ocean indicates major debris inputs from ships
+ View ORCID ProfilePeter G. Ryan, Ben J. Dilley, Robert A. Ronconi, and Maëlle Connan
+PNAS October 15, 2019 116 (42) 20892-20897; first published September 30, 2019 https://doi.org/10.1073/pnas.1909816116</t>
+  </si>
+  <si>
+    <t>https://www.plasticdisclosure.org/solutions</t>
+  </si>
+  <si>
+    <t>Proposed solutions for what becomes of plastic waste</t>
+  </si>
+  <si>
+    <t>http://www.erik.vansebille.com/science/</t>
+  </si>
+  <si>
+    <t>some researcher</t>
+  </si>
+  <si>
+    <t>https://www.theguardian.com/environment/2019/apr/16/six-decade-plankton-study-charts-rise-of-ocean-plastic-waste</t>
+  </si>
+  <si>
+    <t>non-scientific article referencing "The rise in ocean plastics evidenced from a 60-year time series."</t>
+  </si>
+  <si>
+    <t>https://blog.dataiku.com/solving-the-ocean-plastic-pollution-problem-with-data</t>
+  </si>
+  <si>
+    <t>https://www.unenvironment.org/interactive/beat-plastic-pollution/</t>
+  </si>
+  <si>
+    <t>References a few of the papers here (plastic inputs from land, river sources)</t>
+  </si>
+  <si>
+    <t>https://figshare.com/articles/Plastic_Marine_Pollution_Global_Dataset/1015289</t>
+  </si>
+  <si>
+    <t>Plastic Marine Pollution Global Dataset
+Dataset posted on 03.05.2014, 11:14 by Marcus Eriksen
+This is a global dataset of 1571 locations where surface manta tows were conducted.  Samples were divided into 4 size categories. Weights and particle counts were recoreded for each category.</t>
+  </si>
+  <si>
+    <t>Might be a duplicate of georgio's dataset</t>
+  </si>
+  <si>
+    <t>http://www.oceanhealthindex.org/methodology/components/trash-pollution</t>
+  </si>
+  <si>
+    <t>Crawl this page for more sources</t>
+  </si>
+  <si>
+    <t>https://advances.sciencemag.org/content/4/6/eaat0131?intcmp=trendmd-adv&amp;_ga=2.215551700.2143384855.1558607449-269283413.1556900172</t>
+  </si>
+  <si>
+    <t>The Chinese import ban and its impact on global plastic waste trade
+Amy L. Brooks, Shunli Wang and Jenna R. Jambeck*
+ See all authors and affiliations
+Science Advances  20 Jun 2018:
+Vol. 4, no. 6, eaat0131
+DOI: 10.1126/sciadv.aat0131</t>
+  </si>
+  <si>
+    <t>plastic sources</t>
+  </si>
+  <si>
+    <t>https://www.bbc.co.uk/news/uk-46602969</t>
+  </si>
+  <si>
+    <t>The winning international statistic of the year was 90.5% - the proportion of plastic waste that has never been recycled.</t>
+  </si>
+  <si>
+    <t>https://ourworldindata.org/plastic-pollution</t>
   </si>
 </sst>
 </file>
@@ -159,13 +335,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F970D725-1158-44F0-BF8E-E632776E36B3}" name="Table1" displayName="Table1" ref="A1:D7" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A1:D7" xr:uid="{D953BC35-4346-4F2E-81F1-864ECBD1EF34}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F970D725-1158-44F0-BF8E-E632776E36B3}" name="Table1" displayName="Table1" ref="A1:D29" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D29" xr:uid="{D953BC35-4346-4F2E-81F1-864ECBD1EF34}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3A89C75A-D0B3-450A-B68F-59E13523F8A5}" name="Link" dataDxfId="5" dataCellStyle="Hyperlink"/>
-    <tableColumn id="2" xr3:uid="{2EE540E9-7587-4650-A09D-2A46D66570A2}" name="Description" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{30414C29-DBE6-4B68-A206-CFCD4C885551}" name="Notes" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{9431AF31-0BD1-40E2-952C-3C88BC10308D}" name="Poster" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{3A89C75A-D0B3-450A-B68F-59E13523F8A5}" name="Link" dataDxfId="3" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{2EE540E9-7587-4650-A09D-2A46D66570A2}" name="Description" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{30414C29-DBE6-4B68-A206-CFCD4C885551}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{9431AF31-0BD1-40E2-952C-3C88BC10308D}" name="Poster" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -468,19 +644,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84642CED-E167-4D95-A47E-50F339E5EE74}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.21875" defaultRowHeight="38.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="30.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="57.5546875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="30.21875" style="1"/>
+    <col min="2" max="2" width="64.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="35.77734375" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="30.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,7 +672,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -505,7 +683,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -516,7 +694,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -527,7 +705,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -538,7 +716,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -549,7 +727,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -558,6 +736,275 @@
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -568,11 +1015,36 @@
     <hyperlink ref="A5" r:id="rId4" xr:uid="{7BD50F40-F1BF-499D-8794-80BF70E3F29B}"/>
     <hyperlink ref="A6" r:id="rId5" xr:uid="{B9395FAD-F420-4D95-B0BC-1F5288821141}"/>
     <hyperlink ref="A7" r:id="rId6" xr:uid="{6FCD55A5-23B6-4356-AAC0-A95C634273DF}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{49C3C901-922F-4EE8-BC9F-B2B80CF20E75}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{EE632627-D34B-4C13-B2FB-2AD2F769F993}"/>
+    <hyperlink ref="A10" r:id="rId9" location="s5" xr:uid="{22E2407C-6481-4D7A-A8D9-270CE8335321}"/>
+    <hyperlink ref="A12" r:id="rId10" xr:uid="{80D5DA7F-53FB-4677-8AE5-3A8766185A92}"/>
+    <hyperlink ref="A13" r:id="rId11" xr:uid="{3EFE21B9-20E9-4AD9-AAE1-9ABCCC7B3636}"/>
+    <hyperlink ref="A14" r:id="rId12" xr:uid="{48393368-A668-4C26-B7A8-A41B2BF9E654}"/>
+    <hyperlink ref="B8" location="Sources!B14" display="non-scientific article referencing Export of Plastic Debris by Rivers into the Sea" xr:uid="{E66C1064-D246-4837-ABCC-56A62D740CFA}"/>
+    <hyperlink ref="A15" r:id="rId13" xr:uid="{CAF842D9-AF8B-408A-BCCE-E5F81D9E567D}"/>
+    <hyperlink ref="A16" r:id="rId14" xr:uid="{4987C401-2664-4AE4-8510-134CD0D55CA4}"/>
+    <hyperlink ref="A17" r:id="rId15" xr:uid="{44398B50-8E7B-44C5-B195-AF2DD3D946C9}"/>
+    <hyperlink ref="B17" location="Sources!B16" display="non-scientific article referencing &quot;Production, use, and fate of all plastics ever made&quot;" xr:uid="{BE89A222-FA2C-4EA7-9FBC-593FAAAD7402}"/>
+    <hyperlink ref="A18" r:id="rId16" xr:uid="{BAB140BA-B74F-4A67-A11E-18A7A7E4C007}"/>
+    <hyperlink ref="A19" r:id="rId17" xr:uid="{DB84DDAC-9528-42B8-950B-A1FA54A37F42}"/>
+    <hyperlink ref="A11" r:id="rId18" xr:uid="{8FBA29EC-4EBC-41D7-9712-BE078116B874}"/>
+    <hyperlink ref="A20" r:id="rId19" xr:uid="{A53336F5-FE7B-4780-A4F0-E5D600305CCD}"/>
+    <hyperlink ref="A21" r:id="rId20" xr:uid="{11994B1D-52C5-40F4-A133-89ACC2BBF46E}"/>
+    <hyperlink ref="A22" r:id="rId21" xr:uid="{CE19B9D2-6467-44F5-9CED-E74684B21A99}"/>
+    <hyperlink ref="B22" location="Sources!B18" display="non-scientific article referencing &quot;The rise in ocean plastics evidenced from a 60-year time series.&quot;" xr:uid="{81ABCFE7-AEDC-49D1-9046-17EFF2F40170}"/>
+    <hyperlink ref="A23" r:id="rId22" xr:uid="{E2FACB2A-439F-484D-9E62-A940B236205C}"/>
+    <hyperlink ref="A24" r:id="rId23" xr:uid="{83C186F1-F133-4656-B044-47A442BA4BEE}"/>
+    <hyperlink ref="A25" r:id="rId24" xr:uid="{4D1F317E-00D9-4B1B-9B2C-15F083917CF2}"/>
+    <hyperlink ref="A26" r:id="rId25" xr:uid="{474F25F2-2352-4B5F-8A5C-1F52D371094E}"/>
+    <hyperlink ref="A27" r:id="rId26" xr:uid="{14333F07-D547-4FC9-8DDD-816225616284}"/>
+    <hyperlink ref="A28" r:id="rId27" xr:uid="{1373CBC9-8B92-4D7E-B693-A08F705C70FB}"/>
+    <hyperlink ref="A29" r:id="rId28" xr:uid="{CB71DEB9-D8F1-41AF-BF17-D50A9280FD10}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
   <tableParts count="1">
-    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId30"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added new link for plastic debris classification.
</commit_message>
<xml_diff>
--- a/Source Links.xlsx
+++ b/Source Links.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kalyj\OneDrive\RGU\MSc Data Science\CMM507Group2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stuar\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="8_{A19774D1-690D-4199-B5B3-708A58596579}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3F3D3CCB-ABCC-47B5-BFF0-5DF7AF0D37C6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15400C03-AD9F-4617-B335-A90451134492}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="21816" windowHeight="14016" xr2:uid="{DEE519DF-CA73-4E24-A15D-8AAE2AE5105B}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="18426" windowHeight="11746" xr2:uid="{DEE519DF-CA73-4E24-A15D-8AAE2AE5105B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="67">
   <si>
     <t>Link</t>
   </si>
@@ -245,6 +245,15 @@
   </si>
   <si>
     <t>https://ourworldindata.org/plastic-pollution</t>
+  </si>
+  <si>
+    <t>https://marinedebris.engr.uga.edu</t>
+  </si>
+  <si>
+    <t>Debris traking and identification.</t>
+  </si>
+  <si>
+    <t>I will download the collection of plastic data and do some EDA in R.</t>
   </si>
 </sst>
 </file>
@@ -335,8 +344,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F970D725-1158-44F0-BF8E-E632776E36B3}" name="Table1" displayName="Table1" ref="A1:D29" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D29" xr:uid="{D953BC35-4346-4F2E-81F1-864ECBD1EF34}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F970D725-1158-44F0-BF8E-E632776E36B3}" name="Table1" displayName="Table1" ref="A1:D30" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D30" xr:uid="{D953BC35-4346-4F2E-81F1-864ECBD1EF34}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{3A89C75A-D0B3-450A-B68F-59E13523F8A5}" name="Link" dataDxfId="3" dataCellStyle="Hyperlink"/>
     <tableColumn id="2" xr3:uid="{2EE540E9-7587-4650-A09D-2A46D66570A2}" name="Description" dataDxfId="2"/>
@@ -644,21 +653,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84642CED-E167-4D95-A47E-50F339E5EE74}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="F31" sqref="F30:F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="30.234375" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="57.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="64.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="35.77734375" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="30.21875" style="1"/>
+    <col min="1" max="1" width="57.52734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="64.41015625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="35.76171875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="30.234375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -672,7 +681,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -683,7 +692,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -694,7 +703,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -705,7 +714,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -716,7 +725,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -727,7 +736,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -738,7 +747,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -752,7 +761,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="86" x14ac:dyDescent="0.5">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -766,7 +775,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -777,7 +786,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="86" x14ac:dyDescent="0.5">
       <c r="A11" s="2" t="s">
         <v>41</v>
       </c>
@@ -791,7 +800,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -802,7 +811,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="43" x14ac:dyDescent="0.5">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -813,7 +822,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="57.35" x14ac:dyDescent="0.5">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
@@ -827,7 +836,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="43" x14ac:dyDescent="0.5">
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
@@ -841,7 +850,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="57.35" x14ac:dyDescent="0.5">
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
@@ -855,7 +864,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A17" s="2" t="s">
         <v>33</v>
       </c>
@@ -869,7 +878,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="57.35" x14ac:dyDescent="0.5">
       <c r="A18" s="2" t="s">
         <v>35</v>
       </c>
@@ -883,7 +892,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="71.7" x14ac:dyDescent="0.5">
       <c r="A19" s="2" t="s">
         <v>38</v>
       </c>
@@ -897,7 +906,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A20" s="2" t="s">
         <v>44</v>
       </c>
@@ -908,7 +917,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A21" s="2" t="s">
         <v>46</v>
       </c>
@@ -916,7 +925,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A22" s="2" t="s">
         <v>48</v>
       </c>
@@ -927,7 +936,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A23" s="2" t="s">
         <v>50</v>
       </c>
@@ -935,7 +944,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A24" s="2" t="s">
         <v>51</v>
       </c>
@@ -946,7 +955,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="71.7" x14ac:dyDescent="0.5">
       <c r="A25" s="2" t="s">
         <v>53</v>
       </c>
@@ -960,7 +969,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A26" s="2" t="s">
         <v>56</v>
       </c>
@@ -971,7 +980,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="100.35" x14ac:dyDescent="0.5">
       <c r="A27" s="2" t="s">
         <v>58</v>
       </c>
@@ -985,7 +994,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="43" x14ac:dyDescent="0.5">
       <c r="A28" s="2" t="s">
         <v>61</v>
       </c>
@@ -996,7 +1005,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A29" s="2" t="s">
         <v>63</v>
       </c>
@@ -1005,6 +1014,20 @@
       </c>
       <c r="D29" s="1" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A30" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to all files
</commit_message>
<xml_diff>
--- a/Source Links.xlsx
+++ b/Source Links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kalyj\OneDrive\RGU\MSc Data Science\CMM507Group2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="8_{A19774D1-690D-4199-B5B3-708A58596579}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3F3D3CCB-ABCC-47B5-BFF0-5DF7AF0D37C6}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="8_{A19774D1-690D-4199-B5B3-708A58596579}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3ADF4262-7424-45CF-B614-ECA4B110F8B1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="21816" windowHeight="14016" xr2:uid="{DEE519DF-CA73-4E24-A15D-8AAE2AE5105B}"/>
   </bookViews>
@@ -646,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84642CED-E167-4D95-A47E-50F339E5EE74}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
update to source and final project biblitex
</commit_message>
<xml_diff>
--- a/Source Links.xlsx
+++ b/Source Links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kalyj\OneDrive\RGU\MSc Data Science\CMM507Group2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="8_{A19774D1-690D-4199-B5B3-708A58596579}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3ADF4262-7424-45CF-B614-ECA4B110F8B1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="6_{BB720B6E-B34F-4D37-ABD1-3DDF9DD41A5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="21816" windowHeight="14016" xr2:uid="{DEE519DF-CA73-4E24-A15D-8AAE2AE5105B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="67">
   <si>
     <t>Link</t>
   </si>
@@ -245,6 +245,15 @@
   </si>
   <si>
     <t>https://ourworldindata.org/plastic-pollution</t>
+  </si>
+  <si>
+    <t>https://marinedebris.engr.uga.edu</t>
+  </si>
+  <si>
+    <t>Debris traking and identification.</t>
+  </si>
+  <si>
+    <t>I will download the collection of plastic data and do some EDA in R.</t>
   </si>
 </sst>
 </file>
@@ -335,8 +344,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F970D725-1158-44F0-BF8E-E632776E36B3}" name="Table1" displayName="Table1" ref="A1:D29" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D29" xr:uid="{D953BC35-4346-4F2E-81F1-864ECBD1EF34}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F970D725-1158-44F0-BF8E-E632776E36B3}" name="Table1" displayName="Table1" ref="A1:D30" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D30" xr:uid="{D953BC35-4346-4F2E-81F1-864ECBD1EF34}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{3A89C75A-D0B3-450A-B68F-59E13523F8A5}" name="Link" dataDxfId="3" dataCellStyle="Hyperlink"/>
     <tableColumn id="2" xr3:uid="{2EE540E9-7587-4650-A09D-2A46D66570A2}" name="Description" dataDxfId="2"/>
@@ -644,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84642CED-E167-4D95-A47E-50F339E5EE74}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1005,6 +1014,20 @@
       </c>
       <c r="D29" s="1" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
uploads and links from slack
</commit_message>
<xml_diff>
--- a/Source Links.xlsx
+++ b/Source Links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kalyj\OneDrive\RGU\MSc Data Science\CMM507Group2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="6_{BB720B6E-B34F-4D37-ABD1-3DDF9DD41A5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="6_{BB720B6E-B34F-4D37-ABD1-3DDF9DD41A5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{63385F8C-114E-4088-A8F8-B992F4DA8D6D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="21816" windowHeight="14016" xr2:uid="{DEE519DF-CA73-4E24-A15D-8AAE2AE5105B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="72">
   <si>
     <t>Link</t>
   </si>
@@ -254,6 +254,21 @@
   </si>
   <si>
     <t>I will download the collection of plastic data and do some EDA in R.</t>
+  </si>
+  <si>
+    <t>Shipping</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>https://knb.ecoinformatics.org/view/doi:10.5063/F1S180FS</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/331091847_Plastic_Pollution_from_Ships</t>
+  </si>
+  <si>
+    <t>Shipping - The only report that I could find that had any real discussion of data</t>
   </si>
 </sst>
 </file>
@@ -344,8 +359,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F970D725-1158-44F0-BF8E-E632776E36B3}" name="Table1" displayName="Table1" ref="A1:D30" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D30" xr:uid="{D953BC35-4346-4F2E-81F1-864ECBD1EF34}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F970D725-1158-44F0-BF8E-E632776E36B3}" name="Table1" displayName="Table1" ref="A1:D33" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D33" xr:uid="{D953BC35-4346-4F2E-81F1-864ECBD1EF34}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{3A89C75A-D0B3-450A-B68F-59E13523F8A5}" name="Link" dataDxfId="3" dataCellStyle="Hyperlink"/>
     <tableColumn id="2" xr3:uid="{2EE540E9-7587-4650-A09D-2A46D66570A2}" name="Description" dataDxfId="2"/>
@@ -653,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84642CED-E167-4D95-A47E-50F339E5EE74}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1028,6 +1043,39 @@
       </c>
       <c r="D30" s="1" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1063,11 +1111,14 @@
     <hyperlink ref="A27" r:id="rId26" xr:uid="{14333F07-D547-4FC9-8DDD-816225616284}"/>
     <hyperlink ref="A28" r:id="rId27" xr:uid="{1373CBC9-8B92-4D7E-B693-A08F705C70FB}"/>
     <hyperlink ref="A29" r:id="rId28" xr:uid="{CB71DEB9-D8F1-41AF-BF17-D50A9280FD10}"/>
+    <hyperlink ref="A31" r:id="rId29" xr:uid="{D209AE72-2384-4B60-A14B-6268488D1977}"/>
+    <hyperlink ref="A32" r:id="rId30" xr:uid="{34883BC3-8A7C-4212-A03E-4214A7A1B472}"/>
+    <hyperlink ref="A33" r:id="rId31" xr:uid="{B781E737-9ED8-4C74-90CF-923DF46F739F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId32"/>
   <tableParts count="1">
-    <tablePart r:id="rId30"/>
+    <tablePart r:id="rId33"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added link for BBC article - dangers to turtles
</commit_message>
<xml_diff>
--- a/Source Links.xlsx
+++ b/Source Links.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kalyj\OneDrive\RGU\MSc Data Science\CMM507Group2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="6_{BB720B6E-B34F-4D37-ABD1-3DDF9DD41A5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{63385F8C-114E-4088-A8F8-B992F4DA8D6D}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="6_{BB720B6E-B34F-4D37-ABD1-3DDF9DD41A5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B31535B8-E2A8-4928-A7E2-5C8E0EC0B6F7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="21816" windowHeight="14016" xr2:uid="{DEE519DF-CA73-4E24-A15D-8AAE2AE5105B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="75">
   <si>
     <t>Link</t>
   </si>
@@ -269,6 +269,15 @@
   </si>
   <si>
     <t>Shipping - The only report that I could find that had any real discussion of data</t>
+  </si>
+  <si>
+    <t>https://www.bbc.co.uk/news/science-environment-51804884</t>
+  </si>
+  <si>
+    <t>BBC Article: "Why plastic is a deadly attraction for sea turtles"</t>
+  </si>
+  <si>
+    <t>non-scientfic article. Motivations.</t>
   </si>
 </sst>
 </file>
@@ -359,8 +368,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F970D725-1158-44F0-BF8E-E632776E36B3}" name="Table1" displayName="Table1" ref="A1:D33" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D33" xr:uid="{D953BC35-4346-4F2E-81F1-864ECBD1EF34}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F970D725-1158-44F0-BF8E-E632776E36B3}" name="Table1" displayName="Table1" ref="A1:D34" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D34" xr:uid="{D953BC35-4346-4F2E-81F1-864ECBD1EF34}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{3A89C75A-D0B3-450A-B68F-59E13523F8A5}" name="Link" dataDxfId="3" dataCellStyle="Hyperlink"/>
     <tableColumn id="2" xr3:uid="{2EE540E9-7587-4650-A09D-2A46D66570A2}" name="Description" dataDxfId="2"/>
@@ -668,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84642CED-E167-4D95-A47E-50F339E5EE74}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1076,6 +1085,20 @@
       </c>
       <c r="D33" s="1" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1114,11 +1137,12 @@
     <hyperlink ref="A31" r:id="rId29" xr:uid="{D209AE72-2384-4B60-A14B-6268488D1977}"/>
     <hyperlink ref="A32" r:id="rId30" xr:uid="{34883BC3-8A7C-4212-A03E-4214A7A1B472}"/>
     <hyperlink ref="A33" r:id="rId31" xr:uid="{B781E737-9ED8-4C74-90CF-923DF46F739F}"/>
+    <hyperlink ref="A34" r:id="rId32" xr:uid="{3D31820E-ABC1-455B-B3E1-B43538657CE7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId32"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId33"/>
   <tableParts count="1">
-    <tablePart r:id="rId33"/>
+    <tablePart r:id="rId34"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>